<commit_message>
Feature: Added Data Ultis File for common func
</commit_message>
<xml_diff>
--- a/F1Data.xlsx
+++ b/F1Data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P53"/>
+  <dimension ref="A1:P54"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -523,16 +523,16 @@
         <v>9590</v>
       </c>
       <c r="C2" t="n">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D2" t="n">
-        <v>336</v>
+        <v>316</v>
       </c>
       <c r="E2" t="n">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="F2" t="n">
-        <v>279</v>
+        <v>300</v>
       </c>
       <c r="G2" t="inlineStr"/>
       <c r="H2" t="inlineStr"/>
@@ -541,10 +541,10 @@
       </c>
       <c r="J2" t="inlineStr"/>
       <c r="K2" t="n">
-        <v>32.459</v>
+        <v>29.989</v>
       </c>
       <c r="L2" t="n">
-        <v>30.584</v>
+        <v>28.398</v>
       </c>
       <c r="M2" t="inlineStr">
         <is>
@@ -553,12 +553,12 @@
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>[2049, 2049, 2049, 2049, 2049, 2049, 2049]</t>
+          <t>[2049, 2051, 2049, 2049, 2051, 2049, 2049]</t>
         </is>
       </c>
       <c r="O2" t="inlineStr">
         <is>
-          <t>[2049, 2049, 2048, 2049, 2049, 2049, 2049, 2048]</t>
+          <t>[2049, 2048, 2048, 2049, 2049, 2049, 2049, 2049]</t>
         </is>
       </c>
       <c r="P2" t="n">
@@ -573,50 +573,50 @@
         <v>9590</v>
       </c>
       <c r="C3" t="n">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D3" t="n">
-        <v>322</v>
+        <v>315</v>
       </c>
       <c r="E3" t="n">
-        <v>340</v>
+        <v>325</v>
       </c>
       <c r="F3" t="n">
-        <v>340</v>
+        <v>325</v>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>2024-09-01T13:05:10.639000+00:00</t>
+          <t>2024-09-01T13:05:03.005000+00:00</t>
         </is>
       </c>
       <c r="H3" t="n">
-        <v>88.342</v>
+        <v>85.396</v>
       </c>
       <c r="I3" t="b">
         <v>0</v>
       </c>
       <c r="J3" t="n">
-        <v>28.654</v>
+        <v>27.707</v>
       </c>
       <c r="K3" t="n">
-        <v>30.65</v>
+        <v>29.265</v>
       </c>
       <c r="L3" t="n">
-        <v>29.038</v>
+        <v>28.424</v>
       </c>
       <c r="M3" t="inlineStr">
         <is>
-          <t>[2049, 2049, 2049, 2049, 2048, 2048]</t>
+          <t>[2049, 2049, 2049, 2049, 2049, 2049]</t>
         </is>
       </c>
       <c r="N3" t="inlineStr">
         <is>
-          <t>[2049, 2049, 2049, 2049, 2049, 2049, 2051]</t>
+          <t>[2049, 2049, 2051, 2051, 2048, 2049, 2049]</t>
         </is>
       </c>
       <c r="O3" t="inlineStr">
         <is>
-          <t>[2049, 2049, 2048, 2048, 2049, 2049, 2049, 2048]</t>
+          <t>[2048, 2048, 2049, 2048, 2048, 2048, 2048, 2048]</t>
         </is>
       </c>
       <c r="P3" t="n">
@@ -631,50 +631,50 @@
         <v>9590</v>
       </c>
       <c r="C4" t="n">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D4" t="n">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="E4" t="n">
-        <v>340</v>
+        <v>324</v>
       </c>
       <c r="F4" t="n">
-        <v>338</v>
+        <v>328</v>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>2024-09-01T13:06:39.042000+00:00</t>
+          <t>2024-09-01T13:06:28.451000+00:00</t>
         </is>
       </c>
       <c r="H4" t="n">
-        <v>86.73399999999999</v>
+        <v>85.179</v>
       </c>
       <c r="I4" t="b">
         <v>0</v>
       </c>
       <c r="J4" t="n">
-        <v>27.671</v>
+        <v>27.679</v>
       </c>
       <c r="K4" t="n">
-        <v>30.279</v>
+        <v>29.001</v>
       </c>
       <c r="L4" t="n">
-        <v>28.784</v>
+        <v>28.499</v>
       </c>
       <c r="M4" t="inlineStr">
         <is>
-          <t>[None, 2049, 2048, 2049, 2048, 2048]</t>
+          <t>[None, 2049, 2049, 2048, 2049, 2048]</t>
         </is>
       </c>
       <c r="N4" t="inlineStr">
         <is>
-          <t>[2049, 2049, 2049, 2049, 2048, 2048, 2048]</t>
+          <t>[2049, 2049, 2051, 2051, 2048, 2048, 2048]</t>
         </is>
       </c>
       <c r="O4" t="inlineStr">
         <is>
-          <t>[2048, 2049, 2048, 2048, 2049, 2048, 2048, 2048]</t>
+          <t>[2049, 2048, 2049, 2049, 2048, 2048, 2048, 2048]</t>
         </is>
       </c>
       <c r="P4" t="n">
@@ -689,50 +689,50 @@
         <v>9590</v>
       </c>
       <c r="C5" t="n">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D5" t="n">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="E5" t="n">
-        <v>335</v>
+        <v>324</v>
       </c>
       <c r="F5" t="n">
-        <v>344</v>
+        <v>327</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>2024-09-01T13:08:05.802000+00:00</t>
+          <t>2024-09-01T13:07:53.677000+00:00</t>
         </is>
       </c>
       <c r="H5" t="n">
-        <v>86.253</v>
+        <v>84.81</v>
       </c>
       <c r="I5" t="b">
         <v>0</v>
       </c>
       <c r="J5" t="n">
-        <v>27.514</v>
+        <v>27.653</v>
       </c>
       <c r="K5" t="n">
-        <v>29.972</v>
+        <v>28.883</v>
       </c>
       <c r="L5" t="n">
-        <v>28.767</v>
+        <v>28.274</v>
       </c>
       <c r="M5" t="inlineStr">
         <is>
-          <t>[None, 2049, 2048, 2049, 2048, 2048]</t>
+          <t>[None, 2048, 2048, 2048, 2049, 2048]</t>
         </is>
       </c>
       <c r="N5" t="inlineStr">
         <is>
-          <t>[2049, 2049, 2049, 2048, 2049, 2048, 2048]</t>
+          <t>[2049, 2048, 2048, 2051, 2049, 2049, 2048]</t>
         </is>
       </c>
       <c r="O5" t="inlineStr">
         <is>
-          <t>[2048, 2048, 2048, 2048, 2048, 2048, 2048, 2048]</t>
+          <t>[2049, 2048, 2048, 2048, 2049, 2048, 2048, 2048]</t>
         </is>
       </c>
       <c r="P5" t="n">
@@ -747,48 +747,50 @@
         <v>9590</v>
       </c>
       <c r="C6" t="n">
-        <v>18</v>
-      </c>
-      <c r="D6" t="inlineStr"/>
+        <v>16</v>
+      </c>
+      <c r="D6" t="n">
+        <v>313</v>
+      </c>
       <c r="E6" t="n">
-        <v>334</v>
+        <v>325</v>
       </c>
       <c r="F6" t="n">
-        <v>335</v>
+        <v>321</v>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>2024-09-01T13:09:32.041000+00:00</t>
+          <t>2024-09-01T13:09:18.391000+00:00</t>
         </is>
       </c>
       <c r="H6" t="n">
-        <v>87.23399999999999</v>
+        <v>84.60299999999999</v>
       </c>
       <c r="I6" t="b">
         <v>0</v>
       </c>
       <c r="J6" t="n">
-        <v>27.636</v>
+        <v>27.63</v>
       </c>
       <c r="K6" t="n">
-        <v>30.549</v>
+        <v>28.79</v>
       </c>
       <c r="L6" t="n">
-        <v>29.049</v>
+        <v>28.183</v>
       </c>
       <c r="M6" t="inlineStr">
         <is>
-          <t>[2048, 2048, 2048, 2048, 2048, 2048]</t>
+          <t>[2048, 2048, 2049, 2048, 2048, 2048]</t>
         </is>
       </c>
       <c r="N6" t="inlineStr">
         <is>
-          <t>[2048, 2048, 2048, 2049, 2049, 2048, 2048]</t>
+          <t>[2048, 2048, 2048, 2051, 2049, 2049, 2048]</t>
         </is>
       </c>
       <c r="O6" t="inlineStr">
         <is>
-          <t>[2048, 2049, 2048, 2048, 2049, 2049, 2049, 2048]</t>
+          <t>[2049, 2048, 2049, 2049, 2048, 2048, 2048, 2048]</t>
         </is>
       </c>
       <c r="P6" t="n">
@@ -803,48 +805,50 @@
         <v>9590</v>
       </c>
       <c r="C7" t="n">
-        <v>18</v>
-      </c>
-      <c r="D7" t="inlineStr"/>
+        <v>16</v>
+      </c>
+      <c r="D7" t="n">
+        <v>315</v>
+      </c>
       <c r="E7" t="n">
-        <v>330</v>
+        <v>325</v>
       </c>
       <c r="F7" t="n">
-        <v>340</v>
+        <v>325</v>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>2024-09-01T13:10:59.233000+00:00</t>
+          <t>2024-09-01T13:10:43.134000+00:00</t>
         </is>
       </c>
       <c r="H7" t="n">
-        <v>85.55800000000001</v>
+        <v>84.663</v>
       </c>
       <c r="I7" t="b">
         <v>0</v>
       </c>
       <c r="J7" t="n">
-        <v>27.529</v>
+        <v>27.596</v>
       </c>
       <c r="K7" t="n">
-        <v>29.431</v>
+        <v>28.945</v>
       </c>
       <c r="L7" t="n">
-        <v>28.598</v>
+        <v>28.122</v>
       </c>
       <c r="M7" t="inlineStr">
         <is>
-          <t>[None, 2048, 2049, 2049, 2048, 2048]</t>
+          <t>[None, 2049, 2049, 2048, 2048, 2048]</t>
         </is>
       </c>
       <c r="N7" t="inlineStr">
         <is>
-          <t>[2049, 2049, 2049, 2048, 2049, 2048, 2048]</t>
+          <t>[2048, 2048, 2048, 2048, 2049, 2049, 2049]</t>
         </is>
       </c>
       <c r="O7" t="inlineStr">
         <is>
-          <t>[2049, 2049, 2048, 2048, 2049, 2049, 2048, 2048]</t>
+          <t>[2049, 2048, 2049, 2049, 2048, 2048, 2048, 2048]</t>
         </is>
       </c>
       <c r="P7" t="n">
@@ -859,50 +863,50 @@
         <v>9590</v>
       </c>
       <c r="C8" t="n">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D8" t="n">
-        <v>309</v>
+        <v>314</v>
       </c>
       <c r="E8" t="n">
-        <v>315</v>
+        <v>326</v>
       </c>
       <c r="F8" t="n">
-        <v>353</v>
+        <v>329</v>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>2024-09-01T13:12:24.765000+00:00</t>
+          <t>2024-09-01T13:12:07.753000+00:00</t>
         </is>
       </c>
       <c r="H8" t="n">
-        <v>86.208</v>
+        <v>84.434</v>
       </c>
       <c r="I8" t="b">
         <v>0</v>
       </c>
       <c r="J8" t="n">
-        <v>28.114</v>
+        <v>27.645</v>
       </c>
       <c r="K8" t="n">
-        <v>29.553</v>
+        <v>28.701</v>
       </c>
       <c r="L8" t="n">
-        <v>28.541</v>
+        <v>28.088</v>
       </c>
       <c r="M8" t="inlineStr">
         <is>
-          <t>[2049, 2048, 2049, 2048, 2048, 2048]</t>
+          <t>[None, 2048, 2048, 2048, 2048, 2048]</t>
         </is>
       </c>
       <c r="N8" t="inlineStr">
         <is>
-          <t>[2048, 2049, 2049, 2049, 2049, 2048, 2048]</t>
+          <t>[2048, 2048, 2048, 2049, 2049, 2049, 2049]</t>
         </is>
       </c>
       <c r="O8" t="inlineStr">
         <is>
-          <t>[2048, 2048, 2048, 2048, 2048, 2048, 2048, 2048]</t>
+          <t>[2048, 2048, 2048, 2048, 2048, 2048, 2049, 2048]</t>
         </is>
       </c>
       <c r="P8" t="n">
@@ -917,48 +921,48 @@
         <v>9590</v>
       </c>
       <c r="C9" t="n">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D9" t="inlineStr"/>
       <c r="E9" t="n">
-        <v>316</v>
+        <v>325</v>
       </c>
       <c r="F9" t="n">
-        <v>318</v>
+        <v>333</v>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>2024-09-01T13:13:50.899000+00:00</t>
+          <t>2024-09-01T13:13:32.169000+00:00</t>
         </is>
       </c>
       <c r="H9" t="n">
-        <v>85.79900000000001</v>
+        <v>84.569</v>
       </c>
       <c r="I9" t="b">
         <v>0</v>
       </c>
       <c r="J9" t="n">
-        <v>27.799</v>
+        <v>27.557</v>
       </c>
       <c r="K9" t="n">
-        <v>29.379</v>
+        <v>28.771</v>
       </c>
       <c r="L9" t="n">
-        <v>28.621</v>
+        <v>28.241</v>
       </c>
       <c r="M9" t="inlineStr">
         <is>
-          <t>[2048, 2048, 2048, 2049, 2048, 2048]</t>
+          <t>[None, 2049, 2048, 2049, 2048, 2048]</t>
         </is>
       </c>
       <c r="N9" t="inlineStr">
         <is>
-          <t>[2048, 2049, 2048, 2049, 2048, 2048, 2048]</t>
+          <t>[2049, 2048, 2048, 2048, 2048, 2048, 2048]</t>
         </is>
       </c>
       <c r="O9" t="inlineStr">
         <is>
-          <t>[2048, 2048, 2048, 2048, 2048, 2048, 2048, 2048]</t>
+          <t>[2048, 2049, 2049, 2048, 2048, 2048, 2048, 2048]</t>
         </is>
       </c>
       <c r="P9" t="n">
@@ -973,50 +977,46 @@
         <v>9590</v>
       </c>
       <c r="C10" t="n">
-        <v>18</v>
-      </c>
-      <c r="D10" t="n">
-        <v>312</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="D10" t="inlineStr"/>
       <c r="E10" t="n">
-        <v>317</v>
-      </c>
-      <c r="F10" t="n">
-        <v>324</v>
-      </c>
+        <v>326</v>
+      </c>
+      <c r="F10" t="inlineStr"/>
       <c r="G10" t="inlineStr">
         <is>
-          <t>2024-09-01T13:15:16.769000+00:00</t>
+          <t>2024-09-01T13:14:56.660000+00:00</t>
         </is>
       </c>
       <c r="H10" t="n">
-        <v>86.024</v>
+        <v>84.36199999999999</v>
       </c>
       <c r="I10" t="b">
         <v>0</v>
       </c>
       <c r="J10" t="n">
-        <v>27.777</v>
+        <v>27.542</v>
       </c>
       <c r="K10" t="n">
-        <v>29.585</v>
+        <v>28.781</v>
       </c>
       <c r="L10" t="n">
-        <v>28.662</v>
+        <v>28.039</v>
       </c>
       <c r="M10" t="inlineStr">
         <is>
-          <t>[None, 2048, 2048, 2048, 2048, 2048]</t>
+          <t>[2049, 2049, 2048, 2048, 2048, 2048]</t>
         </is>
       </c>
       <c r="N10" t="inlineStr">
         <is>
-          <t>[2048, 2048, 2048, 2048, 2048, 2048, 2048]</t>
+          <t>[2048, 2048, 2048, 2048, 2049, 2049, 2049]</t>
         </is>
       </c>
       <c r="O10" t="inlineStr">
         <is>
-          <t>[2048, 2048, 2048, 2048, 2048, 2048, 2048, 0]</t>
+          <t>[2049, 2049, 2048, 2049, 2048, 2048, 2048, 2048]</t>
         </is>
       </c>
       <c r="P10" t="n">
@@ -1031,50 +1031,48 @@
         <v>9590</v>
       </c>
       <c r="C11" t="n">
-        <v>18</v>
-      </c>
-      <c r="D11" t="n">
-        <v>314</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="D11" t="inlineStr"/>
       <c r="E11" t="n">
-        <v>330</v>
+        <v>325</v>
       </c>
       <c r="F11" t="n">
-        <v>323</v>
+        <v>334</v>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>2024-09-01T13:16:42.750000+00:00</t>
+          <t>2024-09-01T13:16:21.155000+00:00</t>
         </is>
       </c>
       <c r="H11" t="n">
-        <v>86.182</v>
+        <v>84.432</v>
       </c>
       <c r="I11" t="b">
         <v>0</v>
       </c>
       <c r="J11" t="n">
-        <v>27.822</v>
+        <v>27.515</v>
       </c>
       <c r="K11" t="n">
-        <v>29.369</v>
+        <v>28.84</v>
       </c>
       <c r="L11" t="n">
-        <v>28.991</v>
+        <v>28.077</v>
       </c>
       <c r="M11" t="inlineStr">
         <is>
-          <t>[None, 2048, 2048, 2048, 2048, 2048]</t>
+          <t>[2048, 2048, 2049, 2048, 2048, 2048]</t>
         </is>
       </c>
       <c r="N11" t="inlineStr">
         <is>
-          <t>[2048, 2048, 2048, 2049, 2048, 2048, 2048]</t>
+          <t>[2049, 2048, 2048, 2048, 2048, 2048, 2048]</t>
         </is>
       </c>
       <c r="O11" t="inlineStr">
         <is>
-          <t>[2048, 2049, 2048, 2048, 2048, 2048, 2048, 0]</t>
+          <t>[2048, 2048, 2048, 2048, 2048, 2048, 2048, 2048]</t>
         </is>
       </c>
       <c r="P11" t="n">
@@ -1089,36 +1087,36 @@
         <v>9590</v>
       </c>
       <c r="C12" t="n">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D12" t="n">
-        <v>311</v>
+        <v>313</v>
       </c>
       <c r="E12" t="n">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="F12" t="n">
-        <v>329</v>
+        <v>323</v>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>2024-09-01T13:18:08.873000+00:00</t>
+          <t>2024-09-01T13:17:45.559000+00:00</t>
         </is>
       </c>
       <c r="H12" t="n">
-        <v>85.675</v>
+        <v>84.846</v>
       </c>
       <c r="I12" t="b">
         <v>0</v>
       </c>
       <c r="J12" t="n">
-        <v>27.691</v>
+        <v>27.633</v>
       </c>
       <c r="K12" t="n">
-        <v>29.398</v>
+        <v>28.951</v>
       </c>
       <c r="L12" t="n">
-        <v>28.586</v>
+        <v>28.262</v>
       </c>
       <c r="M12" t="inlineStr">
         <is>
@@ -1132,7 +1130,7 @@
       </c>
       <c r="O12" t="inlineStr">
         <is>
-          <t>[2048, 2048, 2048, 2048, 2049, 2049, 2048, 2048]</t>
+          <t>[2048, 2048, 2048, 2048, 2048, 2048, 2048, 2048]</t>
         </is>
       </c>
       <c r="P12" t="n">
@@ -1147,34 +1145,36 @@
         <v>9590</v>
       </c>
       <c r="C13" t="n">
-        <v>18</v>
-      </c>
-      <c r="D13" t="inlineStr"/>
+        <v>16</v>
+      </c>
+      <c r="D13" t="n">
+        <v>312</v>
+      </c>
       <c r="E13" t="n">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="F13" t="n">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>2024-09-01T13:19:34.609000+00:00</t>
+          <t>2024-09-01T13:19:10.276000+00:00</t>
         </is>
       </c>
       <c r="H13" t="n">
-        <v>85.947</v>
+        <v>84.916</v>
       </c>
       <c r="I13" t="b">
         <v>0</v>
       </c>
       <c r="J13" t="n">
-        <v>27.829</v>
+        <v>27.68</v>
       </c>
       <c r="K13" t="n">
-        <v>29.342</v>
+        <v>28.971</v>
       </c>
       <c r="L13" t="n">
-        <v>28.776</v>
+        <v>28.265</v>
       </c>
       <c r="M13" t="inlineStr">
         <is>
@@ -1183,12 +1183,12 @@
       </c>
       <c r="N13" t="inlineStr">
         <is>
-          <t>[2048, 2048, 2049, 2049, 2049, 2048, 2048]</t>
+          <t>[2048, 2048, 2048, 2048, 2048, 2048, 2048]</t>
         </is>
       </c>
       <c r="O13" t="inlineStr">
         <is>
-          <t>[2048, 2048, 2048, 2048, 2048, 2048, 2048, 0]</t>
+          <t>[2048, 2048, 2048, 2048, 2048, 2048, 2048, 2048]</t>
         </is>
       </c>
       <c r="P13" t="n">
@@ -1203,36 +1203,34 @@
         <v>9590</v>
       </c>
       <c r="C14" t="n">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D14" t="n">
-        <v>309</v>
+        <v>311</v>
       </c>
       <c r="E14" t="n">
-        <v>313</v>
-      </c>
-      <c r="F14" t="n">
-        <v>327</v>
-      </c>
+        <v>315</v>
+      </c>
+      <c r="F14" t="inlineStr"/>
       <c r="G14" t="inlineStr">
         <is>
-          <t>2024-09-01T13:21:00.586000+00:00</t>
+          <t>2024-09-01T13:20:35.346000+00:00</t>
         </is>
       </c>
       <c r="H14" t="n">
-        <v>86.143</v>
+        <v>85.529</v>
       </c>
       <c r="I14" t="b">
         <v>0</v>
       </c>
       <c r="J14" t="n">
-        <v>27.742</v>
+        <v>27.812</v>
       </c>
       <c r="K14" t="n">
-        <v>29.697</v>
+        <v>29.177</v>
       </c>
       <c r="L14" t="n">
-        <v>28.704</v>
+        <v>28.54</v>
       </c>
       <c r="M14" t="inlineStr">
         <is>
@@ -1241,12 +1239,12 @@
       </c>
       <c r="N14" t="inlineStr">
         <is>
-          <t>[2048, 2048, 2048, 2048, 2048, 2048, 2048]</t>
+          <t>[2049, 2048, 2048, 2048, 2048, 2048, 2048]</t>
         </is>
       </c>
       <c r="O14" t="inlineStr">
         <is>
-          <t>[2048, 2048, 2048, 2048, 2048, 2048, 2048, 2048]</t>
+          <t>[2049, 2048, 2048, 2048, 2048, 2048, 2048, 2048]</t>
         </is>
       </c>
       <c r="P14" t="n">
@@ -1261,36 +1259,36 @@
         <v>9590</v>
       </c>
       <c r="C15" t="n">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D15" t="n">
+        <v>312</v>
+      </c>
+      <c r="E15" t="n">
         <v>314</v>
-      </c>
-      <c r="E15" t="n">
-        <v>315</v>
       </c>
       <c r="F15" t="n">
         <v>320</v>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>2024-09-01T13:22:26.696000+00:00</t>
+          <t>2024-09-01T13:22:00.856000+00:00</t>
         </is>
       </c>
       <c r="H15" t="n">
-        <v>85.895</v>
+        <v>85.60599999999999</v>
       </c>
       <c r="I15" t="b">
         <v>0</v>
       </c>
       <c r="J15" t="n">
-        <v>27.738</v>
+        <v>27.839</v>
       </c>
       <c r="K15" t="n">
-        <v>29.465</v>
+        <v>29.217</v>
       </c>
       <c r="L15" t="n">
-        <v>28.692</v>
+        <v>28.55</v>
       </c>
       <c r="M15" t="inlineStr">
         <is>
@@ -1299,12 +1297,12 @@
       </c>
       <c r="N15" t="inlineStr">
         <is>
-          <t>[2049, 2048, 2048, 2048, 2048, 2048, 2048]</t>
+          <t>[2048, 2048, 2048, 2048, 2048, 2048, 2048]</t>
         </is>
       </c>
       <c r="O15" t="inlineStr">
         <is>
-          <t>[2048, 2048, 2048, 2048, 2048, 2048, 2048, 2048]</t>
+          <t>[2048, 2048, 2048, 2048, 2048, 2048, 2048, 2064]</t>
         </is>
       </c>
       <c r="P15" t="n">
@@ -1319,36 +1317,34 @@
         <v>9590</v>
       </c>
       <c r="C16" t="n">
-        <v>18</v>
-      </c>
-      <c r="D16" t="n">
-        <v>311</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="D16" t="inlineStr"/>
       <c r="E16" t="n">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="F16" t="n">
         <v>318</v>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>2024-09-01T13:23:52.509000+00:00</t>
+          <t>2024-09-01T13:23:26.425000+00:00</t>
         </is>
       </c>
       <c r="H16" t="n">
-        <v>86.986</v>
+        <v>90.19199999999999</v>
       </c>
       <c r="I16" t="b">
         <v>0</v>
       </c>
       <c r="J16" t="n">
-        <v>28.009</v>
+        <v>28.034</v>
       </c>
       <c r="K16" t="n">
-        <v>29.927</v>
+        <v>29.361</v>
       </c>
       <c r="L16" t="n">
-        <v>29.05</v>
+        <v>32.797</v>
       </c>
       <c r="M16" t="inlineStr">
         <is>
@@ -1362,7 +1358,7 @@
       </c>
       <c r="O16" t="inlineStr">
         <is>
-          <t>[2048, 2048, 2048, 2048, 2048, 2048, 2048, 2048]</t>
+          <t>[2048, 2049, 2049, 2048, 2048, 2048, 2048, 2048]</t>
         </is>
       </c>
       <c r="P16" t="n">
@@ -1377,48 +1373,50 @@
         <v>9590</v>
       </c>
       <c r="C17" t="n">
-        <v>18</v>
-      </c>
-      <c r="D17" t="inlineStr"/>
+        <v>16</v>
+      </c>
+      <c r="D17" t="n">
+        <v>313</v>
+      </c>
       <c r="E17" t="n">
-        <v>311</v>
+        <v>314</v>
       </c>
       <c r="F17" t="n">
-        <v>320</v>
+        <v>284</v>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>2024-09-01T13:25:19.685000+00:00</t>
+          <t>2024-09-01T13:24:56.510000+00:00</t>
         </is>
       </c>
       <c r="H17" t="n">
-        <v>86.593</v>
+        <v>104.888</v>
       </c>
       <c r="I17" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J17" t="n">
-        <v>27.925</v>
+        <v>47.985</v>
       </c>
       <c r="K17" t="n">
-        <v>29.737</v>
+        <v>28.75</v>
       </c>
       <c r="L17" t="n">
-        <v>28.931</v>
+        <v>28.153</v>
       </c>
       <c r="M17" t="inlineStr">
         <is>
-          <t>[None, 2048, 2048, 2048, 2048, 2048]</t>
+          <t>[2064, 2064, 2048, 2049, 2049, 2048]</t>
         </is>
       </c>
       <c r="N17" t="inlineStr">
         <is>
-          <t>[2048, 2048, 2048, 2048, 2048, 2048, 2048]</t>
+          <t>[2048, 2049, 2048, 2048, 2049, 2048, 2048]</t>
         </is>
       </c>
       <c r="O17" t="inlineStr">
         <is>
-          <t>[2048, 2048, 2048, 2048, 2048, 2048, 2048, 2048]</t>
+          <t>[2048, 2048, 2049, 2048, 2048, 2049, 2049, 2049]</t>
         </is>
       </c>
       <c r="P17" t="n">
@@ -1433,48 +1431,50 @@
         <v>9590</v>
       </c>
       <c r="C18" t="n">
-        <v>18</v>
-      </c>
-      <c r="D18" t="inlineStr"/>
+        <v>16</v>
+      </c>
+      <c r="D18" t="n">
+        <v>314</v>
+      </c>
       <c r="E18" t="n">
-        <v>313</v>
+        <v>318</v>
       </c>
       <c r="F18" t="n">
         <v>322</v>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>2024-09-01T13:26:46.146000+00:00</t>
+          <t>2024-09-01T13:26:41.473000+00:00</t>
         </is>
       </c>
       <c r="H18" t="n">
-        <v>86.584</v>
+        <v>84.27</v>
       </c>
       <c r="I18" t="b">
         <v>0</v>
       </c>
       <c r="J18" t="n">
-        <v>27.839</v>
+        <v>27.458</v>
       </c>
       <c r="K18" t="n">
-        <v>29.852</v>
+        <v>28.73</v>
       </c>
       <c r="L18" t="n">
-        <v>28.893</v>
+        <v>28.082</v>
       </c>
       <c r="M18" t="inlineStr">
         <is>
-          <t>[None, 2048, 2048, 2048, 2048, 2048]</t>
+          <t>[2048, 2048, 2049, 2048, 2048, 2049]</t>
         </is>
       </c>
       <c r="N18" t="inlineStr">
         <is>
-          <t>[2048, 2048, 2048, 2048, 2048, 2048, 2048]</t>
+          <t>[2048, 2048, 2048, 2049, 2048, 2048, 2048]</t>
         </is>
       </c>
       <c r="O18" t="inlineStr">
         <is>
-          <t>[2048, 2048, 2048, 2048, 2048, 2048, 2048, 0]</t>
+          <t>[2048, 2049, 2049, 2048, 2048, 2049, 2049, 2049]</t>
         </is>
       </c>
       <c r="P18" t="n">
@@ -1489,50 +1489,50 @@
         <v>9590</v>
       </c>
       <c r="C19" t="n">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D19" t="n">
-        <v>312</v>
+        <v>316</v>
       </c>
       <c r="E19" t="n">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="F19" t="n">
-        <v>325</v>
+        <v>329</v>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>2024-09-01T13:28:12.845000+00:00</t>
+          <t>2024-09-01T13:28:05.665000+00:00</t>
         </is>
       </c>
       <c r="H19" t="n">
-        <v>87.524</v>
+        <v>83.875</v>
       </c>
       <c r="I19" t="b">
         <v>0</v>
       </c>
       <c r="J19" t="n">
-        <v>27.903</v>
+        <v>27.408</v>
       </c>
       <c r="K19" t="n">
-        <v>30.488</v>
+        <v>28.571</v>
       </c>
       <c r="L19" t="n">
-        <v>29.133</v>
+        <v>27.896</v>
       </c>
       <c r="M19" t="inlineStr">
         <is>
-          <t>[None, 2048, 2048, 2048, 2048, 2048]</t>
+          <t>[None, 2048, 2048, 2048, 2048, 2049]</t>
         </is>
       </c>
       <c r="N19" t="inlineStr">
         <is>
-          <t>[2048, 2048, 2048, 2048, 2048, 2048, 2048]</t>
+          <t>[2048, 2048, 2048, 2051, 2048, 2049, 2049]</t>
         </is>
       </c>
       <c r="O19" t="inlineStr">
         <is>
-          <t>[2048, 2048, 2048, 2048, 2048, 2048, 2048, 2064]</t>
+          <t>[2048, 2048, 2048, 2048, 2048, 2048, 2048, 2048]</t>
         </is>
       </c>
       <c r="P19" t="n">
@@ -1547,48 +1547,50 @@
         <v>9590</v>
       </c>
       <c r="C20" t="n">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D20" t="n">
-        <v>314</v>
+        <v>317</v>
       </c>
       <c r="E20" t="n">
-        <v>315</v>
-      </c>
-      <c r="F20" t="inlineStr"/>
+        <v>327</v>
+      </c>
+      <c r="F20" t="n">
+        <v>336</v>
+      </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>2024-09-01T13:29:40.259000+00:00</t>
+          <t>2024-09-01T13:29:29.577000+00:00</t>
         </is>
       </c>
       <c r="H20" t="n">
-        <v>91.321</v>
+        <v>84.203</v>
       </c>
       <c r="I20" t="b">
         <v>0</v>
       </c>
       <c r="J20" t="n">
-        <v>27.867</v>
+        <v>27.354</v>
       </c>
       <c r="K20" t="n">
-        <v>29.83</v>
+        <v>28.722</v>
       </c>
       <c r="L20" t="n">
-        <v>33.624</v>
+        <v>28.127</v>
       </c>
       <c r="M20" t="inlineStr">
         <is>
-          <t>[None, 2048, 2048, 2048, 2048, 2048]</t>
+          <t>[2049, 2049, 2048, 2048, 2049, 2049]</t>
         </is>
       </c>
       <c r="N20" t="inlineStr">
         <is>
-          <t>[2049, 2048, 2048, 2048, 2048, 2048, 2048]</t>
+          <t>[2048, 2048, 2048, 2048, 2048, 2051, 2049]</t>
         </is>
       </c>
       <c r="O20" t="inlineStr">
         <is>
-          <t>[2048, 2048, 2048, 2048, 2049, 2049, 2049, 2048]</t>
+          <t>[2048, 2048, 2048, 2048, 2049, 2049, 2049, 0]</t>
         </is>
       </c>
       <c r="P20" t="n">
@@ -1603,50 +1605,50 @@
         <v>9590</v>
       </c>
       <c r="C21" t="n">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D21" t="n">
-        <v>323</v>
+        <v>315</v>
       </c>
       <c r="E21" t="n">
-        <v>314</v>
+        <v>327</v>
       </c>
       <c r="F21" t="n">
-        <v>283</v>
+        <v>325</v>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>2024-09-01T13:31:11.556000+00:00</t>
+          <t>2024-09-01T13:30:53.769000+00:00</t>
         </is>
       </c>
       <c r="H21" t="n">
-        <v>105.665</v>
+        <v>83.82599999999999</v>
       </c>
       <c r="I21" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J21" t="n">
-        <v>48.081</v>
+        <v>27.483</v>
       </c>
       <c r="K21" t="n">
-        <v>29.135</v>
+        <v>28.623</v>
       </c>
       <c r="L21" t="n">
-        <v>28.449</v>
+        <v>27.72</v>
       </c>
       <c r="M21" t="inlineStr">
         <is>
-          <t>[2064, 2064, 2048, 2048, 2048, 2048]</t>
+          <t>[2048, 2048, 2048, 2048, 2048, 2048]</t>
         </is>
       </c>
       <c r="N21" t="inlineStr">
         <is>
-          <t>[2049, 2048, 2048, 2049, 2049, 2048, 2048]</t>
+          <t>[2048, 2048, 2048, 2048, 2048, 2048, 2048]</t>
         </is>
       </c>
       <c r="O21" t="inlineStr">
         <is>
-          <t>[2049, 2049, 2048, 2048, 2049, 2048, 2048, 2048]</t>
+          <t>[2048, 2049, 2048, 2048, 2048, 2048, 2048, 2048]</t>
         </is>
       </c>
       <c r="P21" t="n">
@@ -1661,50 +1663,48 @@
         <v>9590</v>
       </c>
       <c r="C22" t="n">
-        <v>18</v>
-      </c>
-      <c r="D22" t="n">
-        <v>313</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="D22" t="inlineStr"/>
       <c r="E22" t="n">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="F22" t="n">
-        <v>331</v>
+        <v>335</v>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>2024-09-01T13:32:57.282000+00:00</t>
+          <t>2024-09-01T13:32:17.596000+00:00</t>
         </is>
       </c>
       <c r="H22" t="n">
-        <v>84.721</v>
+        <v>83.88</v>
       </c>
       <c r="I22" t="b">
         <v>0</v>
       </c>
       <c r="J22" t="n">
-        <v>27.443</v>
+        <v>27.423</v>
       </c>
       <c r="K22" t="n">
-        <v>29.024</v>
+        <v>28.725</v>
       </c>
       <c r="L22" t="n">
-        <v>28.254</v>
+        <v>27.732</v>
       </c>
       <c r="M22" t="inlineStr">
         <is>
-          <t>[2048, 2048, 2048, 2049, 2048, 2048]</t>
+          <t>[None, 2048, 2048, 2048, 2049, 2048]</t>
         </is>
       </c>
       <c r="N22" t="inlineStr">
         <is>
-          <t>[2048, 2048, 2049, 2049, 2049, 2048, 2048]</t>
+          <t>[2049, 2048, 2048, 2048, 2048, 2048, 2048]</t>
         </is>
       </c>
       <c r="O22" t="inlineStr">
         <is>
-          <t>[2049, 2049, 2048, 2049, 2049, 2048, 2049, 2048]</t>
+          <t>[2051, 2048, 2048, 2048, 2048, 2048, 2048, 0]</t>
         </is>
       </c>
       <c r="P22" t="n">
@@ -1719,50 +1719,50 @@
         <v>9590</v>
       </c>
       <c r="C23" t="n">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D23" t="n">
         <v>316</v>
       </c>
       <c r="E23" t="n">
-        <v>317</v>
+        <v>328</v>
       </c>
       <c r="F23" t="n">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>2024-09-01T13:34:22.085000+00:00</t>
+          <t>2024-09-01T13:33:41.593000+00:00</t>
         </is>
       </c>
       <c r="H23" t="n">
-        <v>84.721</v>
+        <v>83.768</v>
       </c>
       <c r="I23" t="b">
         <v>0</v>
       </c>
       <c r="J23" t="n">
-        <v>27.515</v>
+        <v>27.358</v>
       </c>
       <c r="K23" t="n">
-        <v>29.053</v>
+        <v>28.484</v>
       </c>
       <c r="L23" t="n">
-        <v>28.153</v>
+        <v>27.926</v>
       </c>
       <c r="M23" t="inlineStr">
         <is>
-          <t>[None, 2048, 2048, 2048, 2049, 2048]</t>
+          <t>[None, 2048, 2048, 2049, 2048, 2048]</t>
         </is>
       </c>
       <c r="N23" t="inlineStr">
         <is>
-          <t>[2048, 2048, 2048, 2049, 2048, 2048, 2048]</t>
+          <t>[2048, 2048, 2048, 2051, 2048, 2048, 2048]</t>
         </is>
       </c>
       <c r="O23" t="inlineStr">
         <is>
-          <t>[2048, 2049, 2048, 2049, 2048, 2048, 2048, 2048]</t>
+          <t>[2048, 2048, 2048, 2048, 2048, 2048, 2048, 2048]</t>
         </is>
       </c>
       <c r="P23" t="n">
@@ -1777,50 +1777,50 @@
         <v>9590</v>
       </c>
       <c r="C24" t="n">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D24" t="n">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="E24" t="n">
-        <v>317</v>
+        <v>319</v>
       </c>
       <c r="F24" t="n">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>2024-09-01T13:35:46.819000+00:00</t>
+          <t>2024-09-01T13:35:05.273000+00:00</t>
         </is>
       </c>
       <c r="H24" t="n">
-        <v>84.65900000000001</v>
+        <v>83.864</v>
       </c>
       <c r="I24" t="b">
         <v>0</v>
       </c>
       <c r="J24" t="n">
-        <v>27.408</v>
+        <v>27.438</v>
       </c>
       <c r="K24" t="n">
-        <v>29.088</v>
+        <v>28.501</v>
       </c>
       <c r="L24" t="n">
-        <v>28.163</v>
+        <v>27.925</v>
       </c>
       <c r="M24" t="inlineStr">
         <is>
-          <t>[None, 2048, 2048, 2048, 2049, 2048]</t>
+          <t>[None, 2048, 2048, 2048, 2048, 2048]</t>
         </is>
       </c>
       <c r="N24" t="inlineStr">
         <is>
-          <t>[2048, 2048, 2048, 2048, 2048, 2048, 2048]</t>
+          <t>[2049, 2049, 2049, 2049, 2048, 2048, 2048]</t>
         </is>
       </c>
       <c r="O24" t="inlineStr">
         <is>
-          <t>[2048, 2048, 2048, 2048, 2048, 2048, 2048, 2048]</t>
+          <t>[2048, 2048, 2048, 2048, 2049, 2048, 2048, 2048]</t>
         </is>
       </c>
       <c r="P24" t="n">
@@ -1835,36 +1835,36 @@
         <v>9590</v>
       </c>
       <c r="C25" t="n">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D25" t="n">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="E25" t="n">
-        <v>317</v>
+        <v>319</v>
       </c>
       <c r="F25" t="n">
         <v>327</v>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>2024-09-01T13:37:11.430000+00:00</t>
+          <t>2024-09-01T13:36:29.098000+00:00</t>
         </is>
       </c>
       <c r="H25" t="n">
-        <v>84.768</v>
+        <v>83.64</v>
       </c>
       <c r="I25" t="b">
         <v>0</v>
       </c>
       <c r="J25" t="n">
-        <v>27.482</v>
+        <v>27.347</v>
       </c>
       <c r="K25" t="n">
-        <v>29.036</v>
+        <v>28.551</v>
       </c>
       <c r="L25" t="n">
-        <v>28.25</v>
+        <v>27.742</v>
       </c>
       <c r="M25" t="inlineStr">
         <is>
@@ -1873,12 +1873,12 @@
       </c>
       <c r="N25" t="inlineStr">
         <is>
-          <t>[2048, 2048, 2049, 2048, 2048, 2048, 2048]</t>
+          <t>[2049, 2048, 2048, 2049, 2048, 2048, 2048]</t>
         </is>
       </c>
       <c r="O25" t="inlineStr">
         <is>
-          <t>[2048, 2048, 2048, 2049, 2048, 2048, 2049, 2048]</t>
+          <t>[2051, 2048, 2048, 2048, 2049, 2048, 2048, 2048]</t>
         </is>
       </c>
       <c r="P25" t="n">
@@ -1893,34 +1893,36 @@
         <v>9590</v>
       </c>
       <c r="C26" t="n">
-        <v>18</v>
-      </c>
-      <c r="D26" t="inlineStr"/>
+        <v>16</v>
+      </c>
+      <c r="D26" t="n">
+        <v>316</v>
+      </c>
       <c r="E26" t="n">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="F26" t="n">
         <v>326</v>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>2024-09-01T13:38:36.196000+00:00</t>
+          <t>2024-09-01T13:37:52.818000+00:00</t>
         </is>
       </c>
       <c r="H26" t="n">
-        <v>84.74299999999999</v>
+        <v>83.59</v>
       </c>
       <c r="I26" t="b">
         <v>0</v>
       </c>
       <c r="J26" t="n">
-        <v>27.401</v>
+        <v>27.38</v>
       </c>
       <c r="K26" t="n">
-        <v>29.097</v>
+        <v>28.445</v>
       </c>
       <c r="L26" t="n">
-        <v>28.245</v>
+        <v>27.765</v>
       </c>
       <c r="M26" t="inlineStr">
         <is>
@@ -1929,12 +1931,12 @@
       </c>
       <c r="N26" t="inlineStr">
         <is>
-          <t>[2048, 2048, 2048, 2048, 2048, 2048, 2048]</t>
+          <t>[2048, 2048, 2049, 2048, 2049, 2048, 2048]</t>
         </is>
       </c>
       <c r="O26" t="inlineStr">
         <is>
-          <t>[2049, 2048, 2048, 2048, 2049, 2048, 2049, 2048]</t>
+          <t>[2048, 2049, 2048, 2048, 2049, 2048, 2049, 2048]</t>
         </is>
       </c>
       <c r="P26" t="n">
@@ -1949,7 +1951,7 @@
         <v>9590</v>
       </c>
       <c r="C27" t="n">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D27" t="inlineStr"/>
       <c r="E27" t="n">
@@ -1960,37 +1962,37 @@
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>2024-09-01T13:40:00.937000+00:00</t>
+          <t>2024-09-01T13:39:16.466000+00:00</t>
         </is>
       </c>
       <c r="H27" t="n">
-        <v>84.491</v>
+        <v>83.321</v>
       </c>
       <c r="I27" t="b">
         <v>0</v>
       </c>
       <c r="J27" t="n">
-        <v>27.491</v>
+        <v>27.356</v>
       </c>
       <c r="K27" t="n">
-        <v>28.9</v>
+        <v>28.307</v>
       </c>
       <c r="L27" t="n">
-        <v>28.1</v>
+        <v>27.658</v>
       </c>
       <c r="M27" t="inlineStr">
         <is>
-          <t>[None, 2048, 2048, 2048, 2048, 2048]</t>
+          <t>[None, 2048, 2048, 2049, 2048, 2048]</t>
         </is>
       </c>
       <c r="N27" t="inlineStr">
         <is>
-          <t>[2049, 2048, 2048, 2048, 2049, 2048, 2048]</t>
+          <t>[2048, 2049, 2048, 2048, 2049, 2048, 2048]</t>
         </is>
       </c>
       <c r="O27" t="inlineStr">
         <is>
-          <t>[2048, 2048, 2048, 2049, 2049, 2048, 2049, 2048]</t>
+          <t>[2048, 2048, 2048, 2048, 2048, 2048, 2049, 2048]</t>
         </is>
       </c>
       <c r="P27" t="n">
@@ -2005,36 +2007,34 @@
         <v>9590</v>
       </c>
       <c r="C28" t="n">
-        <v>18</v>
-      </c>
-      <c r="D28" t="n">
+        <v>16</v>
+      </c>
+      <c r="D28" t="inlineStr"/>
+      <c r="E28" t="n">
         <v>319</v>
       </c>
-      <c r="E28" t="n">
-        <v>330</v>
-      </c>
       <c r="F28" t="n">
-        <v>330</v>
+        <v>325</v>
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>2024-09-01T13:41:25.469000+00:00</t>
+          <t>2024-09-01T13:40:39.849000+00:00</t>
         </is>
       </c>
       <c r="H28" t="n">
-        <v>84.437</v>
+        <v>83.53400000000001</v>
       </c>
       <c r="I28" t="b">
         <v>0</v>
       </c>
       <c r="J28" t="n">
-        <v>27.388</v>
+        <v>27.38</v>
       </c>
       <c r="K28" t="n">
-        <v>28.802</v>
+        <v>28.412</v>
       </c>
       <c r="L28" t="n">
-        <v>28.247</v>
+        <v>27.742</v>
       </c>
       <c r="M28" t="inlineStr">
         <is>
@@ -2043,12 +2043,12 @@
       </c>
       <c r="N28" t="inlineStr">
         <is>
-          <t>[2048, 2048, 2048, 2048, 2048, 2048, 2048]</t>
+          <t>[2049, 2048, 2048, 2048, 2049, 2048, 2048]</t>
         </is>
       </c>
       <c r="O28" t="inlineStr">
         <is>
-          <t>[2048, 2048, 2048, 2049, 2048, 2048, 2049, 2048]</t>
+          <t>[2048, 2049, 2049, 2048, 2048, 2048, 2048, 2048]</t>
         </is>
       </c>
       <c r="P28" t="n">
@@ -2063,48 +2063,50 @@
         <v>9590</v>
       </c>
       <c r="C29" t="n">
-        <v>18</v>
-      </c>
-      <c r="D29" t="inlineStr"/>
+        <v>16</v>
+      </c>
+      <c r="D29" t="n">
+        <v>317</v>
+      </c>
       <c r="E29" t="n">
-        <v>331</v>
+        <v>320</v>
       </c>
       <c r="F29" t="n">
-        <v>345</v>
+        <v>326</v>
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>2024-09-01T13:42:49.841000+00:00</t>
+          <t>2024-09-01T13:42:03.253000+00:00</t>
         </is>
       </c>
       <c r="H29" t="n">
-        <v>84.61799999999999</v>
+        <v>83.28400000000001</v>
       </c>
       <c r="I29" t="b">
         <v>0</v>
       </c>
       <c r="J29" t="n">
-        <v>27.371</v>
+        <v>27.337</v>
       </c>
       <c r="K29" t="n">
-        <v>28.965</v>
+        <v>28.297</v>
       </c>
       <c r="L29" t="n">
-        <v>28.282</v>
+        <v>27.65</v>
       </c>
       <c r="M29" t="inlineStr">
         <is>
-          <t>[None, 2048, 2048, 2048, 2049, 2048]</t>
+          <t>[None, 2048, 2048, 2049, 2049, 2048]</t>
         </is>
       </c>
       <c r="N29" t="inlineStr">
         <is>
-          <t>[2048, 2048, 2049, 2048, 2048, 2048, 2048]</t>
+          <t>[2048, 2048, 2048, 2049, 2048, 2048, 2048]</t>
         </is>
       </c>
       <c r="O29" t="inlineStr">
         <is>
-          <t>[2048, 2048, 2048, 2048, 2048, 2048, 2049, 2049]</t>
+          <t>[2048, 2048, 2049, 2048, 2049, 2048, 2049, 2048]</t>
         </is>
       </c>
       <c r="P29" t="n">
@@ -2119,50 +2121,48 @@
         <v>9590</v>
       </c>
       <c r="C30" t="n">
-        <v>18</v>
-      </c>
-      <c r="D30" t="n">
-        <v>322</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="D30" t="inlineStr"/>
       <c r="E30" t="n">
-        <v>335</v>
+        <v>319</v>
       </c>
       <c r="F30" t="n">
-        <v>339</v>
+        <v>325</v>
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>2024-09-01T13:44:14.531000+00:00</t>
+          <t>2024-09-01T13:43:26.515000+00:00</t>
         </is>
       </c>
       <c r="H30" t="n">
-        <v>85.39700000000001</v>
+        <v>83.229</v>
       </c>
       <c r="I30" t="b">
         <v>0</v>
       </c>
       <c r="J30" t="n">
-        <v>27.362</v>
+        <v>27.336</v>
       </c>
       <c r="K30" t="n">
-        <v>29.444</v>
+        <v>28.301</v>
       </c>
       <c r="L30" t="n">
-        <v>28.591</v>
+        <v>27.592</v>
       </c>
       <c r="M30" t="inlineStr">
         <is>
-          <t>[None, 2048, 2048, 2048, 2049, 2048]</t>
+          <t>[None, 2048, 2048, 2048, 2048, 2048]</t>
         </is>
       </c>
       <c r="N30" t="inlineStr">
         <is>
-          <t>[2048, 2048, 2048, 2048, 2048, 2049, 2048]</t>
+          <t>[2048, 2048, 2048, 2048, 2049, 2048, 2048]</t>
         </is>
       </c>
       <c r="O30" t="inlineStr">
         <is>
-          <t>[2048, 2048, 2049, 2048, 2048, 2048, 2049, 0]</t>
+          <t>[2048, 2048, 2049, 2048, 2048, 2048, 2048, 2048]</t>
         </is>
       </c>
       <c r="P30" t="n">
@@ -2177,50 +2177,46 @@
         <v>9590</v>
       </c>
       <c r="C31" t="n">
-        <v>18</v>
-      </c>
-      <c r="D31" t="n">
-        <v>331</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="D31" t="inlineStr"/>
       <c r="E31" t="n">
-        <v>336</v>
-      </c>
-      <c r="F31" t="n">
-        <v>342</v>
-      </c>
+        <v>320</v>
+      </c>
+      <c r="F31" t="inlineStr"/>
       <c r="G31" t="inlineStr">
         <is>
-          <t>2024-09-01T13:45:39.907000+00:00</t>
+          <t>2024-09-01T13:44:49.738000+00:00</t>
         </is>
       </c>
       <c r="H31" t="n">
-        <v>86.377</v>
+        <v>83.35899999999999</v>
       </c>
       <c r="I31" t="b">
         <v>0</v>
       </c>
       <c r="J31" t="n">
-        <v>27.631</v>
+        <v>27.361</v>
       </c>
       <c r="K31" t="n">
-        <v>29.905</v>
+        <v>28.259</v>
       </c>
       <c r="L31" t="n">
-        <v>28.841</v>
+        <v>27.739</v>
       </c>
       <c r="M31" t="inlineStr">
         <is>
-          <t>[2049, 2049, 2048, 2048, 2049, 2049]</t>
+          <t>[None, 2048, 2048, 2048, 2048, 2048]</t>
         </is>
       </c>
       <c r="N31" t="inlineStr">
         <is>
-          <t>[2048, 2048, 2048, 2048, 2048, 2049, 2048]</t>
+          <t>[2048, 2049, 2049, 2048, 2048, 2048, 2048]</t>
         </is>
       </c>
       <c r="O31" t="inlineStr">
         <is>
-          <t>[2048, 2048, 2048, 2048, 2048, 2048, 2048, 2048]</t>
+          <t>[2048, 2048, 2049, 2048, 2048, 2049, 2049, 0]</t>
         </is>
       </c>
       <c r="P31" t="n">
@@ -2235,50 +2231,50 @@
         <v>9590</v>
       </c>
       <c r="C32" t="n">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D32" t="n">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="E32" t="n">
-        <v>336</v>
+        <v>329</v>
       </c>
       <c r="F32" t="n">
-        <v>340</v>
+        <v>326</v>
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>2024-09-01T13:47:06.223000+00:00</t>
+          <t>2024-09-01T13:46:13.093000+00:00</t>
         </is>
       </c>
       <c r="H32" t="n">
-        <v>84.749</v>
+        <v>83.97199999999999</v>
       </c>
       <c r="I32" t="b">
         <v>0</v>
       </c>
       <c r="J32" t="n">
-        <v>27.379</v>
+        <v>27.312</v>
       </c>
       <c r="K32" t="n">
-        <v>29.025</v>
+        <v>28.74</v>
       </c>
       <c r="L32" t="n">
-        <v>28.345</v>
+        <v>27.92</v>
       </c>
       <c r="M32" t="inlineStr">
         <is>
-          <t>[2048, 2048, 2048, 2048, 2048, 2048]</t>
+          <t>[None, 2048, 2048, 2048, 2048, 2048]</t>
         </is>
       </c>
       <c r="N32" t="inlineStr">
         <is>
-          <t>[2048, 2048, 2048, 2048, 2048, 2049, 2048]</t>
+          <t>[2048, 2049, 2048, 2048, 2048, 2049, 2049]</t>
         </is>
       </c>
       <c r="O32" t="inlineStr">
         <is>
-          <t>[2048, 2048, 2048, 2048, 2048, 2048, 2048, 2048]</t>
+          <t>[2048, 2048, 2049, 2048, 2048, 2048, 2048, 2048]</t>
         </is>
       </c>
       <c r="P32" t="n">
@@ -2293,43 +2289,45 @@
         <v>9590</v>
       </c>
       <c r="C33" t="n">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D33" t="n">
-        <v>327</v>
+        <v>319</v>
       </c>
       <c r="E33" t="n">
         <v>331</v>
       </c>
-      <c r="F33" t="inlineStr"/>
+      <c r="F33" t="n">
+        <v>338</v>
+      </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>2024-09-01T13:48:31.057000+00:00</t>
+          <t>2024-09-01T13:47:37.075000+00:00</t>
         </is>
       </c>
       <c r="H33" t="n">
-        <v>85.57599999999999</v>
+        <v>83.274</v>
       </c>
       <c r="I33" t="b">
         <v>0</v>
       </c>
       <c r="J33" t="n">
-        <v>27.675</v>
+        <v>27.246</v>
       </c>
       <c r="K33" t="n">
-        <v>29.483</v>
+        <v>28.382</v>
       </c>
       <c r="L33" t="n">
-        <v>28.418</v>
+        <v>27.646</v>
       </c>
       <c r="M33" t="inlineStr">
         <is>
-          <t>[None, 2048, 2048, 2048, 2048, 2048]</t>
+          <t>[2049, 2049, 2048, 2048, 2049, 2049]</t>
         </is>
       </c>
       <c r="N33" t="inlineStr">
         <is>
-          <t>[2048, 2048, 2049, 2048, 2048, 2048, 2048]</t>
+          <t>[2048, 2048, 2048, 2048, 2048, 2048, 2049]</t>
         </is>
       </c>
       <c r="O33" t="inlineStr">
@@ -2349,50 +2347,50 @@
         <v>9590</v>
       </c>
       <c r="C34" t="n">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D34" t="n">
         <v>315</v>
       </c>
       <c r="E34" t="n">
-        <v>329</v>
+        <v>319</v>
       </c>
       <c r="F34" t="n">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>2024-09-01T13:49:56.555000+00:00</t>
+          <t>2024-09-01T13:49:00.302000+00:00</t>
         </is>
       </c>
       <c r="H34" t="n">
-        <v>84.947</v>
+        <v>83.226</v>
       </c>
       <c r="I34" t="b">
         <v>0</v>
       </c>
       <c r="J34" t="n">
-        <v>27.546</v>
+        <v>27.189</v>
       </c>
       <c r="K34" t="n">
-        <v>29.102</v>
+        <v>28.364</v>
       </c>
       <c r="L34" t="n">
-        <v>28.299</v>
+        <v>27.673</v>
       </c>
       <c r="M34" t="inlineStr">
         <is>
-          <t>[None, 2048, 2048, 2048, 2048, 2048]</t>
+          <t>[2048, 2048, 2048, 2049, 2048, 2048]</t>
         </is>
       </c>
       <c r="N34" t="inlineStr">
         <is>
-          <t>[2048, 2048, 2048, 2048, 2048, 2048, 2048]</t>
+          <t>[2049, 2048, 2048, 2048, 2048, 2048, 2048]</t>
         </is>
       </c>
       <c r="O34" t="inlineStr">
         <is>
-          <t>[2048, 2048, 2048, 2049, 2048, 2048, 2048, 2048]</t>
+          <t>[2048, 2048, 2048, 2048, 2048, 2048, 2048, 2048]</t>
         </is>
       </c>
       <c r="P34" t="n">
@@ -2407,36 +2405,36 @@
         <v>9590</v>
       </c>
       <c r="C35" t="n">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D35" t="n">
-        <v>321</v>
+        <v>316</v>
       </c>
       <c r="E35" t="n">
-        <v>332</v>
+        <v>320</v>
       </c>
       <c r="F35" t="n">
-        <v>343</v>
+        <v>325</v>
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>2024-09-01T13:51:21.614000+00:00</t>
+          <t>2024-09-01T13:50:23.556000+00:00</t>
         </is>
       </c>
       <c r="H35" t="n">
-        <v>84.85599999999999</v>
+        <v>83.43000000000001</v>
       </c>
       <c r="I35" t="b">
         <v>0</v>
       </c>
       <c r="J35" t="n">
-        <v>27.349</v>
+        <v>27.324</v>
       </c>
       <c r="K35" t="n">
-        <v>29.1</v>
+        <v>28.408</v>
       </c>
       <c r="L35" t="n">
-        <v>28.407</v>
+        <v>27.698</v>
       </c>
       <c r="M35" t="inlineStr">
         <is>
@@ -2450,7 +2448,7 @@
       </c>
       <c r="O35" t="inlineStr">
         <is>
-          <t>[2048, 2048, 2048, 2048, 2048, 2048, 2048, 2048]</t>
+          <t>[2048, 2048, 2049, 2048, 2048, 2048, 2048, 2048]</t>
         </is>
       </c>
       <c r="P35" t="n">
@@ -2465,34 +2463,32 @@
         <v>9590</v>
       </c>
       <c r="C36" t="n">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D36" t="inlineStr"/>
       <c r="E36" t="n">
-        <v>331</v>
-      </c>
-      <c r="F36" t="n">
-        <v>339</v>
-      </c>
+        <v>319</v>
+      </c>
+      <c r="F36" t="inlineStr"/>
       <c r="G36" t="inlineStr">
         <is>
-          <t>2024-09-01T13:52:46.565000+00:00</t>
+          <t>2024-09-01T13:51:47.042000+00:00</t>
         </is>
       </c>
       <c r="H36" t="n">
-        <v>84.863</v>
+        <v>83.681</v>
       </c>
       <c r="I36" t="b">
         <v>0</v>
       </c>
       <c r="J36" t="n">
-        <v>27.402</v>
+        <v>27.393</v>
       </c>
       <c r="K36" t="n">
-        <v>29.095</v>
+        <v>28.512</v>
       </c>
       <c r="L36" t="n">
-        <v>28.366</v>
+        <v>27.776</v>
       </c>
       <c r="M36" t="inlineStr">
         <is>
@@ -2501,12 +2497,12 @@
       </c>
       <c r="N36" t="inlineStr">
         <is>
-          <t>[2048, 2048, 2049, 2048, 2048, 2048, 2048]</t>
+          <t>[2048, 2048, 2048, 2048, 2048, 2048, 2048]</t>
         </is>
       </c>
       <c r="O36" t="inlineStr">
         <is>
-          <t>[2048, 2048, 2048, 2048, 2048, 2048, 2048, 2064]</t>
+          <t>[2048, 2048, 2048, 2048, 2048, 2048, 2048, 2048]</t>
         </is>
       </c>
       <c r="P36" t="n">
@@ -2521,36 +2517,34 @@
         <v>9590</v>
       </c>
       <c r="C37" t="n">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D37" t="n">
         <v>318</v>
       </c>
       <c r="E37" t="n">
-        <v>330</v>
-      </c>
-      <c r="F37" t="n">
-        <v>337</v>
-      </c>
+        <v>321</v>
+      </c>
+      <c r="F37" t="inlineStr"/>
       <c r="G37" t="inlineStr">
         <is>
-          <t>2024-09-01T13:54:11.274000+00:00</t>
+          <t>2024-09-01T13:53:10.810000+00:00</t>
         </is>
       </c>
       <c r="H37" t="n">
-        <v>89.334</v>
+        <v>83.714</v>
       </c>
       <c r="I37" t="b">
         <v>0</v>
       </c>
       <c r="J37" t="n">
-        <v>27.44</v>
+        <v>27.31</v>
       </c>
       <c r="K37" t="n">
-        <v>29.135</v>
+        <v>28.493</v>
       </c>
       <c r="L37" t="n">
-        <v>32.759</v>
+        <v>27.911</v>
       </c>
       <c r="M37" t="inlineStr">
         <is>
@@ -2564,7 +2558,7 @@
       </c>
       <c r="O37" t="inlineStr">
         <is>
-          <t>[2048, 2049, 2048, 2048, 2049, 2049, 2049, 2048]</t>
+          <t>[2049, 2048, 2048, 2048, 2048, 2048, 2048, 2048]</t>
         </is>
       </c>
       <c r="P37" t="n">
@@ -2579,40 +2573,40 @@
         <v>9590</v>
       </c>
       <c r="C38" t="n">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D38" t="n">
-        <v>328</v>
+        <v>316</v>
       </c>
       <c r="E38" t="n">
-        <v>325</v>
+        <v>319</v>
       </c>
       <c r="F38" t="n">
-        <v>283</v>
+        <v>335</v>
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>2024-09-01T13:55:40.455000+00:00</t>
+          <t>2024-09-01T13:54:34.446000+00:00</t>
         </is>
       </c>
       <c r="H38" t="n">
-        <v>103.775</v>
+        <v>83.55</v>
       </c>
       <c r="I38" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J38" t="n">
-        <v>46.949</v>
+        <v>27.279</v>
       </c>
       <c r="K38" t="n">
-        <v>28.823</v>
+        <v>28.457</v>
       </c>
       <c r="L38" t="n">
-        <v>28.003</v>
+        <v>27.814</v>
       </c>
       <c r="M38" t="inlineStr">
         <is>
-          <t>[2064, 2064, 2048, 2048, 2048, 2048]</t>
+          <t>[None, 2048, 2048, 2048, 2048, 2048]</t>
         </is>
       </c>
       <c r="N38" t="inlineStr">
@@ -2622,7 +2616,7 @@
       </c>
       <c r="O38" t="inlineStr">
         <is>
-          <t>[2048, 2049, 2048, 2048, 2049, 2049, 2048, 0]</t>
+          <t>[2048, 2049, 2048, 2048, 2048, 2048, 2048, 2048]</t>
         </is>
       </c>
       <c r="P38" t="n">
@@ -2637,50 +2631,50 @@
         <v>9590</v>
       </c>
       <c r="C39" t="n">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D39" t="n">
-        <v>313</v>
+        <v>318</v>
       </c>
       <c r="E39" t="n">
-        <v>315</v>
+        <v>320</v>
       </c>
       <c r="F39" t="n">
-        <v>356</v>
+        <v>325</v>
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>2024-09-01T13:57:24.361000+00:00</t>
+          <t>2024-09-01T13:55:57.904000+00:00</t>
         </is>
       </c>
       <c r="H39" t="n">
-        <v>83.617</v>
+        <v>83.624</v>
       </c>
       <c r="I39" t="b">
         <v>0</v>
       </c>
       <c r="J39" t="n">
-        <v>26.947</v>
+        <v>27.372</v>
       </c>
       <c r="K39" t="n">
-        <v>28.796</v>
+        <v>28.466</v>
       </c>
       <c r="L39" t="n">
-        <v>27.874</v>
+        <v>27.786</v>
       </c>
       <c r="M39" t="inlineStr">
         <is>
-          <t>[2048, 2048, 2051, 2048, 2048, 2048]</t>
+          <t>[None, 2048, 2048, 2048, 2048, 2048]</t>
         </is>
       </c>
       <c r="N39" t="inlineStr">
         <is>
-          <t>[2048, 2049, 2048, 2048, 2049, 2048, 2048]</t>
+          <t>[2048, 2048, 2048, 2048, 2048, 2048, 2048]</t>
         </is>
       </c>
       <c r="O39" t="inlineStr">
         <is>
-          <t>[2048, 2048, 2048, 2048, 2048, 2048, 2048, 2049]</t>
+          <t>[2048, 2049, 2048, 2048, 2048, 2048, 2048, 2048]</t>
         </is>
       </c>
       <c r="P39" t="n">
@@ -2695,40 +2689,36 @@
         <v>9590</v>
       </c>
       <c r="C40" t="n">
-        <v>18</v>
-      </c>
-      <c r="D40" t="n">
-        <v>314</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="D40" t="inlineStr"/>
       <c r="E40" t="n">
-        <v>330</v>
-      </c>
-      <c r="F40" t="n">
-        <v>324</v>
-      </c>
+        <v>327</v>
+      </c>
+      <c r="F40" t="inlineStr"/>
       <c r="G40" t="inlineStr">
         <is>
-          <t>2024-09-01T13:58:47.897000+00:00</t>
+          <t>2024-09-01T13:57:21.606000+00:00</t>
         </is>
       </c>
       <c r="H40" t="n">
-        <v>84.43000000000001</v>
+        <v>83.718</v>
       </c>
       <c r="I40" t="b">
         <v>0</v>
       </c>
       <c r="J40" t="n">
-        <v>27.336</v>
+        <v>27.448</v>
       </c>
       <c r="K40" t="n">
-        <v>28.607</v>
+        <v>28.564</v>
       </c>
       <c r="L40" t="n">
-        <v>28.487</v>
+        <v>27.706</v>
       </c>
       <c r="M40" t="inlineStr">
         <is>
-          <t>[None, 2048, 2048, 2049, 2048, 2048]</t>
+          <t>[None, 2048, 2048, 2048, 2048, 2048]</t>
         </is>
       </c>
       <c r="N40" t="inlineStr">
@@ -2738,7 +2728,7 @@
       </c>
       <c r="O40" t="inlineStr">
         <is>
-          <t>[2048, 2048, 2049, 2048, 2048, 2048, 2048, 2049]</t>
+          <t>[2051, 2048, 2048, 2048, 2048, 2048, 2048, 0]</t>
         </is>
       </c>
       <c r="P40" t="n">
@@ -2753,40 +2743,40 @@
         <v>9590</v>
       </c>
       <c r="C41" t="n">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D41" t="n">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="E41" t="n">
-        <v>331</v>
+        <v>318</v>
       </c>
       <c r="F41" t="n">
-        <v>356</v>
+        <v>322</v>
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>2024-09-01T14:00:12.478000+00:00</t>
+          <t>2024-09-01T13:58:45.324000+00:00</t>
         </is>
       </c>
       <c r="H41" t="n">
-        <v>85.777</v>
+        <v>83.69</v>
       </c>
       <c r="I41" t="b">
         <v>0</v>
       </c>
       <c r="J41" t="n">
-        <v>28.301</v>
+        <v>27.399</v>
       </c>
       <c r="K41" t="n">
-        <v>28.853</v>
+        <v>28.465</v>
       </c>
       <c r="L41" t="n">
-        <v>28.623</v>
+        <v>27.826</v>
       </c>
       <c r="M41" t="inlineStr">
         <is>
-          <t>[None, 2048, 2051, 2048, 2048, 2048]</t>
+          <t>[None, 2048, 2048, 2048, 2048, 2048]</t>
         </is>
       </c>
       <c r="N41" t="inlineStr">
@@ -2796,7 +2786,7 @@
       </c>
       <c r="O41" t="inlineStr">
         <is>
-          <t>[2048, 2049, 2048, 2048, 2049, 2048, 2048, 0]</t>
+          <t>[2048, 2048, 2048, 2048, 2048, 2048, 2048, 2048]</t>
         </is>
       </c>
       <c r="P41" t="n">
@@ -2811,36 +2801,32 @@
         <v>9590</v>
       </c>
       <c r="C42" t="n">
-        <v>18</v>
-      </c>
-      <c r="D42" t="n">
-        <v>311</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="D42" t="inlineStr"/>
       <c r="E42" t="n">
-        <v>312</v>
-      </c>
-      <c r="F42" t="n">
-        <v>355</v>
-      </c>
+        <v>318</v>
+      </c>
+      <c r="F42" t="inlineStr"/>
       <c r="G42" t="inlineStr">
         <is>
-          <t>2024-09-01T14:01:38.245000+00:00</t>
+          <t>2024-09-01T14:00:08.946000+00:00</t>
         </is>
       </c>
       <c r="H42" t="n">
-        <v>83.702</v>
+        <v>83.611</v>
       </c>
       <c r="I42" t="b">
         <v>0</v>
       </c>
       <c r="J42" t="n">
-        <v>26.975</v>
+        <v>27.372</v>
       </c>
       <c r="K42" t="n">
-        <v>28.741</v>
+        <v>28.44</v>
       </c>
       <c r="L42" t="n">
-        <v>27.986</v>
+        <v>27.799</v>
       </c>
       <c r="M42" t="inlineStr">
         <is>
@@ -2849,12 +2835,12 @@
       </c>
       <c r="N42" t="inlineStr">
         <is>
-          <t>[2048, 2048, 2048, 2049, 2049, 2048, 2048]</t>
+          <t>[2048, 2048, 2048, 2048, 2048, 2048, 2048]</t>
         </is>
       </c>
       <c r="O42" t="inlineStr">
         <is>
-          <t>[2048, 2049, 2048, 2048, 2049, 2049, 2048, 2048]</t>
+          <t>[2048, 2048, 2049, 2048, 2048, 2048, 2048, 2048]</t>
         </is>
       </c>
       <c r="P42" t="n">
@@ -2869,36 +2855,36 @@
         <v>9590</v>
       </c>
       <c r="C43" t="n">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D43" t="n">
-        <v>312</v>
+        <v>316</v>
       </c>
       <c r="E43" t="n">
-        <v>313</v>
+        <v>319</v>
       </c>
       <c r="F43" t="n">
-        <v>319</v>
+        <v>323</v>
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>2024-09-01T14:03:01.766000+00:00</t>
+          <t>2024-09-01T14:01:32.637000+00:00</t>
         </is>
       </c>
       <c r="H43" t="n">
-        <v>83.82299999999999</v>
+        <v>83.67</v>
       </c>
       <c r="I43" t="b">
         <v>0</v>
       </c>
       <c r="J43" t="n">
-        <v>27.461</v>
+        <v>27.424</v>
       </c>
       <c r="K43" t="n">
-        <v>28.549</v>
+        <v>28.458</v>
       </c>
       <c r="L43" t="n">
-        <v>27.813</v>
+        <v>27.788</v>
       </c>
       <c r="M43" t="inlineStr">
         <is>
@@ -2907,12 +2893,12 @@
       </c>
       <c r="N43" t="inlineStr">
         <is>
-          <t>[2048, 2048, 2049, 2049, 2049, 2048, 2048]</t>
+          <t>[2048, 2048, 2049, 2048, 2048, 2048, 2048]</t>
         </is>
       </c>
       <c r="O43" t="inlineStr">
         <is>
-          <t>[2048, 2049, 2048, 2048, 2049, 2048, 2048, 2048]</t>
+          <t>[2048, 2048, 2049, 2048, 2048, 2048, 2048, 2048]</t>
         </is>
       </c>
       <c r="P43" t="n">
@@ -2927,34 +2913,36 @@
         <v>9590</v>
       </c>
       <c r="C44" t="n">
-        <v>18</v>
-      </c>
-      <c r="D44" t="inlineStr"/>
+        <v>16</v>
+      </c>
+      <c r="D44" t="n">
+        <v>318</v>
+      </c>
       <c r="E44" t="n">
-        <v>314</v>
+        <v>321</v>
       </c>
       <c r="F44" t="n">
-        <v>322</v>
+        <v>324</v>
       </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t>2024-09-01T14:04:25.665000+00:00</t>
+          <t>2024-09-01T14:02:56.287000+00:00</t>
         </is>
       </c>
       <c r="H44" t="n">
-        <v>83.81</v>
+        <v>83.867</v>
       </c>
       <c r="I44" t="b">
         <v>0</v>
       </c>
       <c r="J44" t="n">
-        <v>27.534</v>
+        <v>27.382</v>
       </c>
       <c r="K44" t="n">
-        <v>28.496</v>
+        <v>28.558</v>
       </c>
       <c r="L44" t="n">
-        <v>27.78</v>
+        <v>27.927</v>
       </c>
       <c r="M44" t="inlineStr">
         <is>
@@ -2963,12 +2951,12 @@
       </c>
       <c r="N44" t="inlineStr">
         <is>
-          <t>[2048, 2048, 2049, 2049, 2048, 2048, 2048]</t>
+          <t>[2048, 2048, 2048, 2048, 2048, 2048, 2048]</t>
         </is>
       </c>
       <c r="O44" t="inlineStr">
         <is>
-          <t>[2048, 2048, 2048, 2048, 2048, 2048, 2049, 2048]</t>
+          <t>[2048, 2049, 2048, 2048, 2048, 2048, 2048, 2048]</t>
         </is>
       </c>
       <c r="P44" t="n">
@@ -2983,36 +2971,36 @@
         <v>9590</v>
       </c>
       <c r="C45" t="n">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D45" t="n">
         <v>315</v>
       </c>
       <c r="E45" t="n">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="F45" t="n">
-        <v>321</v>
+        <v>323</v>
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>2024-09-01T14:05:49.536000+00:00</t>
+          <t>2024-09-01T14:04:20.156000+00:00</t>
         </is>
       </c>
       <c r="H45" t="n">
-        <v>83.654</v>
+        <v>83.43000000000001</v>
       </c>
       <c r="I45" t="b">
         <v>0</v>
       </c>
       <c r="J45" t="n">
-        <v>27.358</v>
+        <v>27.386</v>
       </c>
       <c r="K45" t="n">
-        <v>28.411</v>
+        <v>28.395</v>
       </c>
       <c r="L45" t="n">
-        <v>27.885</v>
+        <v>27.649</v>
       </c>
       <c r="M45" t="inlineStr">
         <is>
@@ -3021,12 +3009,12 @@
       </c>
       <c r="N45" t="inlineStr">
         <is>
-          <t>[2049, 2048, 2049, 2049, 2048, 2048, 2048]</t>
+          <t>[2048, 2048, 2048, 2048, 2048, 2048, 2048]</t>
         </is>
       </c>
       <c r="O45" t="inlineStr">
         <is>
-          <t>[2048, 2049, 2048, 2048, 2048, 2049, 2049, 2048]</t>
+          <t>[2048, 2048, 2048, 2048, 2048, 2048, 2048, 2048]</t>
         </is>
       </c>
       <c r="P45" t="n">
@@ -3041,36 +3029,36 @@
         <v>9590</v>
       </c>
       <c r="C46" t="n">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D46" t="n">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="E46" t="n">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="F46" t="n">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="G46" t="inlineStr">
         <is>
-          <t>2024-09-01T14:07:13.193000+00:00</t>
+          <t>2024-09-01T14:05:43.646000+00:00</t>
         </is>
       </c>
       <c r="H46" t="n">
-        <v>83.42700000000001</v>
+        <v>83.73099999999999</v>
       </c>
       <c r="I46" t="b">
         <v>0</v>
       </c>
       <c r="J46" t="n">
-        <v>27.348</v>
+        <v>27.507</v>
       </c>
       <c r="K46" t="n">
-        <v>28.321</v>
+        <v>28.427</v>
       </c>
       <c r="L46" t="n">
-        <v>27.758</v>
+        <v>27.797</v>
       </c>
       <c r="M46" t="inlineStr">
         <is>
@@ -3079,7 +3067,7 @@
       </c>
       <c r="N46" t="inlineStr">
         <is>
-          <t>[2048, 2049, 2049, 2048, 2048, 2048, 2048]</t>
+          <t>[2048, 2048, 2048, 2048, 2048, 2048, 2048]</t>
         </is>
       </c>
       <c r="O46" t="inlineStr">
@@ -3099,43 +3087,45 @@
         <v>9590</v>
       </c>
       <c r="C47" t="n">
-        <v>18</v>
-      </c>
-      <c r="D47" t="inlineStr"/>
+        <v>16</v>
+      </c>
+      <c r="D47" t="n">
+        <v>316</v>
+      </c>
       <c r="E47" t="n">
-        <v>317</v>
+        <v>319</v>
       </c>
       <c r="F47" t="n">
         <v>323</v>
       </c>
       <c r="G47" t="inlineStr">
         <is>
-          <t>2024-09-01T14:08:36.612000+00:00</t>
+          <t>2024-09-01T14:07:07.289000+00:00</t>
         </is>
       </c>
       <c r="H47" t="n">
-        <v>83.90600000000001</v>
+        <v>83.59699999999999</v>
       </c>
       <c r="I47" t="b">
         <v>0</v>
       </c>
       <c r="J47" t="n">
-        <v>27.371</v>
+        <v>27.539</v>
       </c>
       <c r="K47" t="n">
-        <v>28.627</v>
+        <v>28.364</v>
       </c>
       <c r="L47" t="n">
-        <v>27.908</v>
+        <v>27.694</v>
       </c>
       <c r="M47" t="inlineStr">
         <is>
-          <t>[None, 2048, 2048, 2048, 2048, 2048]</t>
+          <t>[None, 2048, 2049, 2048, 2048, 2048]</t>
         </is>
       </c>
       <c r="N47" t="inlineStr">
         <is>
-          <t>[2048, 2048, 2048, 2048, 2048, 2048, 2048]</t>
+          <t>[2048, 2048, 2049, 2048, 2048, 2048, 2048]</t>
         </is>
       </c>
       <c r="O47" t="inlineStr">
@@ -3155,36 +3145,36 @@
         <v>9590</v>
       </c>
       <c r="C48" t="n">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D48" t="n">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="E48" t="n">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="F48" t="n">
-        <v>326</v>
+        <v>321</v>
       </c>
       <c r="G48" t="inlineStr">
         <is>
-          <t>2024-09-01T14:10:00.546000+00:00</t>
+          <t>2024-09-01T14:08:30.866000+00:00</t>
         </is>
       </c>
       <c r="H48" t="n">
-        <v>84.014</v>
+        <v>83.676</v>
       </c>
       <c r="I48" t="b">
         <v>0</v>
       </c>
       <c r="J48" t="n">
-        <v>27.349</v>
+        <v>27.509</v>
       </c>
       <c r="K48" t="n">
-        <v>28.673</v>
+        <v>28.426</v>
       </c>
       <c r="L48" t="n">
-        <v>27.992</v>
+        <v>27.741</v>
       </c>
       <c r="M48" t="inlineStr">
         <is>
@@ -3198,7 +3188,7 @@
       </c>
       <c r="O48" t="inlineStr">
         <is>
-          <t>[2048, 2048, 2048, 2048, 2048, 2048, 2048, 2048]</t>
+          <t>[2048, 2048, 2048, 2048, 2048, 2049, 2049, 2048]</t>
         </is>
       </c>
       <c r="P48" t="n">
@@ -3213,34 +3203,34 @@
         <v>9590</v>
       </c>
       <c r="C49" t="n">
-        <v>18</v>
-      </c>
-      <c r="D49" t="n">
-        <v>317</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="D49" t="inlineStr"/>
       <c r="E49" t="n">
-        <v>291</v>
-      </c>
-      <c r="F49" t="inlineStr"/>
+        <v>318</v>
+      </c>
+      <c r="F49" t="n">
+        <v>322</v>
+      </c>
       <c r="G49" t="inlineStr">
         <is>
-          <t>2024-09-01T14:11:24.524000+00:00</t>
+          <t>2024-09-01T14:09:54.613000+00:00</t>
         </is>
       </c>
       <c r="H49" t="n">
-        <v>86.104</v>
+        <v>83.518</v>
       </c>
       <c r="I49" t="b">
         <v>0</v>
       </c>
       <c r="J49" t="n">
-        <v>27.419</v>
+        <v>27.502</v>
       </c>
       <c r="K49" t="n">
-        <v>29.351</v>
+        <v>28.365</v>
       </c>
       <c r="L49" t="n">
-        <v>29.334</v>
+        <v>27.651</v>
       </c>
       <c r="M49" t="inlineStr">
         <is>
@@ -3254,7 +3244,7 @@
       </c>
       <c r="O49" t="inlineStr">
         <is>
-          <t>[2048, 2048, 2048, 2048, 2048, 2048, 2048, 2048]</t>
+          <t>[2048, 2048, 2048, 2048, 2048, 2048, 2049, 2048]</t>
         </is>
       </c>
       <c r="P49" t="n">
@@ -3269,34 +3259,34 @@
         <v>9590</v>
       </c>
       <c r="C50" t="n">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D50" t="n">
-        <v>314</v>
+        <v>316</v>
       </c>
       <c r="E50" t="n">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="F50" t="inlineStr"/>
       <c r="G50" t="inlineStr">
         <is>
-          <t>2024-09-01T14:12:50.685000+00:00</t>
+          <t>2024-09-01T14:11:18.153000+00:00</t>
         </is>
       </c>
       <c r="H50" t="n">
-        <v>85.06399999999999</v>
+        <v>83.467</v>
       </c>
       <c r="I50" t="b">
         <v>0</v>
       </c>
       <c r="J50" t="n">
-        <v>27.468</v>
+        <v>27.457</v>
       </c>
       <c r="K50" t="n">
-        <v>29.129</v>
+        <v>28.319</v>
       </c>
       <c r="L50" t="n">
-        <v>28.467</v>
+        <v>27.691</v>
       </c>
       <c r="M50" t="inlineStr">
         <is>
@@ -3310,7 +3300,7 @@
       </c>
       <c r="O50" t="inlineStr">
         <is>
-          <t>[2048, 2048, 2048, 2048, 2048, 2048, 2048, 2064]</t>
+          <t>[2048, 2048, 2048, 2048, 2048, 2048, 2048, 2048]</t>
         </is>
       </c>
       <c r="P50" t="n">
@@ -3325,36 +3315,32 @@
         <v>9590</v>
       </c>
       <c r="C51" t="n">
-        <v>18</v>
-      </c>
-      <c r="D51" t="n">
-        <v>321</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="D51" t="inlineStr"/>
       <c r="E51" t="n">
         <v>318</v>
       </c>
-      <c r="F51" t="n">
-        <v>320</v>
-      </c>
+      <c r="F51" t="inlineStr"/>
       <c r="G51" t="inlineStr">
         <is>
-          <t>2024-09-01T14:14:15.757000+00:00</t>
+          <t>2024-09-01T14:12:41.531000+00:00</t>
         </is>
       </c>
       <c r="H51" t="n">
-        <v>90.18600000000001</v>
+        <v>83.461</v>
       </c>
       <c r="I51" t="b">
         <v>0</v>
       </c>
       <c r="J51" t="n">
-        <v>27.901</v>
+        <v>27.425</v>
       </c>
       <c r="K51" t="n">
-        <v>29.194</v>
+        <v>28.336</v>
       </c>
       <c r="L51" t="n">
-        <v>33.091</v>
+        <v>27.7</v>
       </c>
       <c r="M51" t="inlineStr">
         <is>
@@ -3368,7 +3354,7 @@
       </c>
       <c r="O51" t="inlineStr">
         <is>
-          <t>[2048, 2048, 2048, 2048, 2048, 2049, 2049, 2048]</t>
+          <t>[2048, 2048, 2049, 2048, 2048, 2048, 2049, 2048]</t>
         </is>
       </c>
       <c r="P51" t="n">
@@ -3383,50 +3369,50 @@
         <v>9590</v>
       </c>
       <c r="C52" t="n">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D52" t="n">
-        <v>265</v>
+        <v>318</v>
       </c>
       <c r="E52" t="n">
-        <v>318</v>
+        <v>320</v>
       </c>
       <c r="F52" t="n">
-        <v>247</v>
+        <v>323</v>
       </c>
       <c r="G52" t="inlineStr">
         <is>
-          <t>2024-09-01T14:15:45.956000+00:00</t>
+          <t>2024-09-01T14:14:05.018000+00:00</t>
         </is>
       </c>
       <c r="H52" t="n">
-        <v>110.98</v>
+        <v>83.55500000000001</v>
       </c>
       <c r="I52" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J52" t="n">
-        <v>49.959</v>
+        <v>27.432</v>
       </c>
       <c r="K52" t="n">
-        <v>32.44</v>
+        <v>28.386</v>
       </c>
       <c r="L52" t="n">
-        <v>28.581</v>
+        <v>27.737</v>
       </c>
       <c r="M52" t="inlineStr">
         <is>
-          <t>[2064, 2064, 2048, 2048, 2048, 2048]</t>
+          <t>[None, 2048, 2048, 2048, 2048, 2048]</t>
         </is>
       </c>
       <c r="N52" t="inlineStr">
         <is>
-          <t>[2048, 2048, 2048, 2048, 2048, 2048, 2048]</t>
+          <t>[2048, 2048, 2049, 2048, 2048, 2048, 2048]</t>
         </is>
       </c>
       <c r="O52" t="inlineStr">
         <is>
-          <t>[2049, 2049, 2049, 2048, 2049, 2048, 2049, 2048]</t>
+          <t>[2048, 2048, 2048, 2048, 2048, 2048, 2048, 2048]</t>
         </is>
       </c>
       <c r="P52" t="n">
@@ -3441,54 +3427,112 @@
         <v>9590</v>
       </c>
       <c r="C53" t="n">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D53" t="n">
+        <v>319</v>
+      </c>
+      <c r="E53" t="n">
+        <v>321</v>
+      </c>
+      <c r="F53" t="n">
         <v>324</v>
       </c>
-      <c r="E53" t="n">
-        <v>319</v>
-      </c>
-      <c r="F53" t="n">
-        <v>337</v>
-      </c>
       <c r="G53" t="inlineStr">
         <is>
-          <t>2024-09-01T14:17:36.874000+00:00</t>
+          <t>2024-09-01T14:15:28.694000+00:00</t>
         </is>
       </c>
       <c r="H53" t="n">
-        <v>82.232</v>
+        <v>83.75</v>
       </c>
       <c r="I53" t="b">
         <v>0</v>
       </c>
       <c r="J53" t="n">
-        <v>26.932</v>
+        <v>27.432</v>
       </c>
       <c r="K53" t="n">
-        <v>27.914</v>
+        <v>28.471</v>
       </c>
       <c r="L53" t="n">
-        <v>27.386</v>
+        <v>27.847</v>
       </c>
       <c r="M53" t="inlineStr">
         <is>
-          <t>[2048, 2048, 2048, 2049, 2048, 2048]</t>
+          <t>[None, 2048, 2048, 2048, 2049, 2049]</t>
         </is>
       </c>
       <c r="N53" t="inlineStr">
         <is>
-          <t>[2049, 2049, 2049, 2049, 2049, 2049, 2048]</t>
+          <t>[2048, 2048, 2049, 2048, 2048, 2048, 2048]</t>
         </is>
       </c>
       <c r="O53" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[2049, 2048, 2049, 2048, 2048, 2048, 2048, 0]</t>
         </is>
       </c>
       <c r="P53" t="n">
         <v>52</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="n">
+        <v>1244</v>
+      </c>
+      <c r="B54" t="n">
+        <v>9590</v>
+      </c>
+      <c r="C54" t="n">
+        <v>16</v>
+      </c>
+      <c r="D54" t="n">
+        <v>324</v>
+      </c>
+      <c r="E54" t="n">
+        <v>326</v>
+      </c>
+      <c r="F54" t="n">
+        <v>329</v>
+      </c>
+      <c r="G54" t="inlineStr">
+        <is>
+          <t>2024-09-01T14:16:52.392000+00:00</t>
+        </is>
+      </c>
+      <c r="H54" t="n">
+        <v>83.268</v>
+      </c>
+      <c r="I54" t="b">
+        <v>0</v>
+      </c>
+      <c r="J54" t="n">
+        <v>27.285</v>
+      </c>
+      <c r="K54" t="n">
+        <v>28.302</v>
+      </c>
+      <c r="L54" t="n">
+        <v>27.681</v>
+      </c>
+      <c r="M54" t="inlineStr">
+        <is>
+          <t>[None, 2048, 2048, 2048, 2049, 2049]</t>
+        </is>
+      </c>
+      <c r="N54" t="inlineStr">
+        <is>
+          <t>[2048, 2048, 2049, 2048, 2048, 2048, 2048]</t>
+        </is>
+      </c>
+      <c r="O54" t="inlineStr">
+        <is>
+          <t>[0, 0, 0, 0, 0, 0, 0, 0]</t>
+        </is>
+      </c>
+      <c r="P54" t="n">
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>